<commit_message>
review and standardize styling
</commit_message>
<xml_diff>
--- a/docs/tables.xlsx
+++ b/docs/tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsalvatore/Dropbox (University of Michigan)/projects/dissertation/aim_one/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47267E53-1CE0-F842-8195-A355E38D4DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB9D1E4-0404-E149-9644-BCDC4B851727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{B83973B1-1A22-9546-8AE4-1199476E5C00}"/>
   </bookViews>
@@ -843,16 +843,16 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1172,7 +1172,7 @@
   <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1183,12 +1183,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="20"/>
@@ -2155,44 +2155,44 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="34" customHeight="1">
-      <c r="A70" s="36" t="s">
+      <c r="A70" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
     </row>
     <row r="71" spans="1:4" ht="16" customHeight="1">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="36"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="33" t="s">
+      <c r="A72" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B72" s="33"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="C73" s="33"/>
-      <c r="D73" s="33"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
     </row>
     <row r="74" spans="1:4" ht="32" customHeight="1">
-      <c r="A74" s="33" t="s">
+      <c r="A74" s="36" t="s">
         <v>204</v>
       </c>
-      <c r="B74" s="33"/>
-      <c r="C74" s="33"/>
-      <c r="D74" s="33"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
sync phecode prev comp script
</commit_message>
<xml_diff>
--- a/docs/tables.xlsx
+++ b/docs/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsalvatore/Dropbox (University of Michigan)/projects/dissertation/aim_one/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A8AFA5-6891-DA40-B48B-1456140C354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24444ABE-9DB4-B94B-AE95-5B6C26D6BD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{B83973B1-1A22-9546-8AE4-1199476E5C00}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{B83973B1-1A22-9546-8AE4-1199476E5C00}"/>
   </bookViews>
   <sheets>
     <sheet name="table 1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="483">
   <si>
     <t>MGI</t>
   </si>
@@ -2058,6 +2058,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2075,12 +2081,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2399,7 +2399,7 @@
   <dimension ref="A1:O76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2419,20 +2419,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="35" customHeight="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>389</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
     </row>
     <row r="2" spans="1:12" ht="19">
       <c r="A2" s="20"/>
@@ -2445,13 +2445,13 @@
       <c r="D2" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="22" t="s">
         <v>247</v>
       </c>
       <c r="H2" s="22" t="s">
@@ -3517,8 +3517,9 @@
         <v>29.1 (0.2)</v>
       </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24" t="s">
-        <v>157</v>
+      <c r="J31" s="24" t="str">
+        <f>ukb_unweighted!C21</f>
+        <v>27.43 (4.80)</v>
       </c>
       <c r="K31" s="24" t="str">
         <f>ukb_weighted!E18</f>
@@ -3563,8 +3564,9 @@
         <f>nhanes_weighted!E23</f>
         <v xml:space="preserve"> 3.2 (0.2)</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>157</v>
+      <c r="J33" s="4" t="str">
+        <f>ukb_unweighted!C26</f>
+        <v xml:space="preserve"> 0.5 (2,610)</v>
       </c>
       <c r="K33" s="4" t="str">
         <f>ukb_weighted!E22</f>
@@ -3606,8 +3608,9 @@
         <f>nhanes_weighted!E20</f>
         <v>27.9 (1.2)</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>157</v>
+      <c r="J34" s="4" t="str">
+        <f>ukb_unweighted!C23</f>
+        <v>32.5 (161,476)</v>
       </c>
       <c r="K34" s="4" t="str">
         <f>ukb_weighted!E19</f>
@@ -3649,8 +3652,9 @@
         <f>nhanes_weighted!E22</f>
         <v>29.6 (1.1)</v>
       </c>
-      <c r="J35" s="4" t="s">
-        <v>157</v>
+      <c r="J35" s="4" t="str">
+        <f>ukb_unweighted!C22</f>
+        <v>42.5 (211,358)</v>
       </c>
       <c r="K35" s="4" t="str">
         <f>ukb_weighted!E21</f>
@@ -3692,8 +3696,9 @@
         <f>nhanes_weighted!E21</f>
         <v>39.3 (1.6)</v>
       </c>
-      <c r="J36" s="4" t="s">
-        <v>157</v>
+      <c r="J36" s="4" t="str">
+        <f>ukb_unweighted!C25</f>
+        <v>24.5 (121,629)</v>
       </c>
       <c r="K36" s="4" t="str">
         <f>ukb_weighted!E20</f>
@@ -4137,7 +4142,7 @@
       <c r="D50" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="E50" s="24">
+      <c r="E50" s="51">
         <f>aou_unweighted!C44</f>
         <v>1</v>
       </c>
@@ -4176,7 +4181,7 @@
       <c r="D51" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="E51" s="24">
+      <c r="E51" s="51">
         <f>aou_unweighted!C45</f>
         <v>17</v>
       </c>
@@ -4215,7 +4220,7 @@
       <c r="D52" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="E52" s="24">
+      <c r="E52" s="51">
         <f>aou_unweighted!C46</f>
         <v>30</v>
       </c>
@@ -4254,7 +4259,7 @@
       <c r="D53" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="E53" s="24">
+      <c r="E53" s="51">
         <f>aou_unweighted!C47</f>
         <v>481</v>
       </c>
@@ -4678,7 +4683,7 @@
       <c r="A65" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="56">
+      <c r="B65" s="50">
         <f>mgi_unweighted!C59</f>
         <v>0</v>
       </c>
@@ -4688,7 +4693,7 @@
       <c r="D65" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E65" s="56">
+      <c r="E65" s="50">
         <f>aou_unweighted!C60</f>
         <v>0</v>
       </c>
@@ -4727,7 +4732,7 @@
       <c r="D66" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E66" s="56">
+      <c r="E66" s="50">
         <f>aou_unweighted!C61</f>
         <v>7</v>
       </c>
@@ -4766,7 +4771,7 @@
       <c r="D67" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E67" s="56">
+      <c r="E67" s="50">
         <f>aou_unweighted!C62</f>
         <v>9</v>
       </c>
@@ -4805,7 +4810,7 @@
       <c r="D68" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="E68" s="56">
+      <c r="E68" s="50">
         <f>aou_unweighted!C63</f>
         <v>41</v>
       </c>
@@ -4831,132 +4836,132 @@
       </c>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="53" t="s">
+      <c r="A69" s="55" t="s">
         <v>250</v>
       </c>
-      <c r="B69" s="53"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="53"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="53"/>
-      <c r="G69" s="53"/>
-      <c r="H69" s="53"/>
-      <c r="I69" s="53"/>
-      <c r="J69" s="53"/>
-      <c r="K69" s="53"/>
-      <c r="L69" s="53"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="55"/>
+      <c r="I69" s="55"/>
+      <c r="J69" s="55"/>
+      <c r="K69" s="55"/>
+      <c r="L69" s="55"/>
     </row>
     <row r="70" spans="1:12" ht="16" customHeight="1">
-      <c r="A70" s="51" t="s">
+      <c r="A70" s="53" t="s">
         <v>248</v>
       </c>
-      <c r="B70" s="54"/>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="54"/>
-      <c r="G70" s="54"/>
-      <c r="H70" s="54"/>
-      <c r="I70" s="54"/>
-      <c r="J70" s="54"/>
-      <c r="K70" s="54"/>
-      <c r="L70" s="54"/>
+      <c r="B70" s="56"/>
+      <c r="C70" s="56"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="56"/>
+      <c r="G70" s="56"/>
+      <c r="H70" s="56"/>
+      <c r="I70" s="56"/>
+      <c r="J70" s="56"/>
+      <c r="K70" s="56"/>
+      <c r="L70" s="56"/>
     </row>
     <row r="71" spans="1:12" ht="35" customHeight="1">
-      <c r="A71" s="51" t="s">
+      <c r="A71" s="53" t="s">
         <v>385</v>
       </c>
-      <c r="B71" s="51"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="51"/>
-      <c r="F71" s="51"/>
-      <c r="G71" s="51"/>
-      <c r="H71" s="51"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="51"/>
-      <c r="K71" s="51"/>
-      <c r="L71" s="51"/>
+      <c r="B71" s="53"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="53"/>
+      <c r="I71" s="53"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="53"/>
+      <c r="L71" s="53"/>
     </row>
     <row r="72" spans="1:12" ht="33" customHeight="1">
-      <c r="A72" s="51" t="s">
+      <c r="A72" s="53" t="s">
         <v>259</v>
       </c>
-      <c r="B72" s="51"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="51"/>
-      <c r="G72" s="51"/>
-      <c r="H72" s="51"/>
-      <c r="I72" s="51"/>
-      <c r="J72" s="51"/>
-      <c r="K72" s="51"/>
-      <c r="L72" s="51"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="53"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="53"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="53"/>
+      <c r="K72" s="53"/>
+      <c r="L72" s="53"/>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="51" t="s">
+      <c r="A73" s="53" t="s">
         <v>386</v>
       </c>
-      <c r="B73" s="54"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="54"/>
-      <c r="E73" s="54"/>
-      <c r="F73" s="54"/>
-      <c r="G73" s="54"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="54"/>
-      <c r="J73" s="54"/>
-      <c r="K73" s="54"/>
-      <c r="L73" s="54"/>
+      <c r="B73" s="56"/>
+      <c r="C73" s="56"/>
+      <c r="D73" s="56"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="56"/>
+      <c r="G73" s="56"/>
+      <c r="H73" s="56"/>
+      <c r="I73" s="56"/>
+      <c r="J73" s="56"/>
+      <c r="K73" s="56"/>
+      <c r="L73" s="56"/>
     </row>
     <row r="74" spans="1:12" ht="16" customHeight="1">
-      <c r="A74" s="51" t="s">
+      <c r="A74" s="53" t="s">
         <v>387</v>
       </c>
-      <c r="B74" s="54"/>
-      <c r="C74" s="54"/>
-      <c r="D74" s="54"/>
-      <c r="E74" s="54"/>
-      <c r="F74" s="54"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="54"/>
-      <c r="K74" s="54"/>
-      <c r="L74" s="54"/>
+      <c r="B74" s="56"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="56"/>
+      <c r="G74" s="56"/>
+      <c r="H74" s="56"/>
+      <c r="I74" s="56"/>
+      <c r="J74" s="56"/>
+      <c r="K74" s="56"/>
+      <c r="L74" s="56"/>
     </row>
     <row r="75" spans="1:12" ht="22" customHeight="1">
-      <c r="A75" s="51" t="s">
+      <c r="A75" s="53" t="s">
         <v>388</v>
       </c>
-      <c r="B75" s="54"/>
-      <c r="C75" s="54"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="54"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="54"/>
-      <c r="I75" s="54"/>
-      <c r="J75" s="54"/>
-      <c r="K75" s="54"/>
-      <c r="L75" s="54"/>
+      <c r="B75" s="56"/>
+      <c r="C75" s="56"/>
+      <c r="D75" s="56"/>
+      <c r="E75" s="56"/>
+      <c r="F75" s="56"/>
+      <c r="G75" s="56"/>
+      <c r="H75" s="56"/>
+      <c r="I75" s="56"/>
+      <c r="J75" s="56"/>
+      <c r="K75" s="56"/>
+      <c r="L75" s="56"/>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="50" t="s">
+      <c r="A76" s="52" t="s">
         <v>251</v>
       </c>
-      <c r="B76" s="50"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
-      <c r="E76" s="50"/>
-      <c r="F76" s="50"/>
-      <c r="G76" s="50"/>
-      <c r="H76" s="50"/>
-      <c r="I76" s="50"/>
-      <c r="J76" s="50"/>
-      <c r="K76" s="50"/>
-      <c r="L76" s="50"/>
+      <c r="B76" s="52"/>
+      <c r="C76" s="52"/>
+      <c r="D76" s="52"/>
+      <c r="E76" s="52"/>
+      <c r="F76" s="52"/>
+      <c r="G76" s="52"/>
+      <c r="H76" s="52"/>
+      <c r="I76" s="52"/>
+      <c r="J76" s="52"/>
+      <c r="K76" s="52"/>
+      <c r="L76" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -10389,11 +10394,11 @@
       <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="57" t="s">
         <v>262</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:5" ht="17">
       <c r="A3" s="39" t="s">

</xml_diff>